<commit_message>
wip: update redux state when option selected
</commit_message>
<xml_diff>
--- a/notes/notes - doors quote generator.xlsx
+++ b/notes/notes - doors quote generator.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AApps\door-quote-automator\notes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10500" windowHeight="6450" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10500" windowHeight="6450" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
     <sheet name="Notes" sheetId="3" r:id="rId2"/>
-    <sheet name="Door quote vs plugin" sheetId="4" r:id="rId3"/>
+    <sheet name="Catefories" sheetId="5" r:id="rId3"/>
+    <sheet name="Door quote vs plugin" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -21,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
   <si>
     <t>v 0.1</t>
   </si>
@@ -215,11 +221,50 @@
   <si>
     <t>A branding header with MEK Logo and Contact number</t>
   </si>
+  <si>
+    <t>Single Door Options</t>
+  </si>
+  <si>
+    <t>Glass - 02 options</t>
+  </si>
+  <si>
+    <t>Double Door</t>
+  </si>
+  <si>
+    <t>Height, input box</t>
+  </si>
+  <si>
+    <t>Width, input box</t>
+  </si>
+  <si>
+    <t>door closer</t>
+  </si>
+  <si>
+    <t>louver required</t>
+  </si>
+  <si>
+    <t>Door Type(Fire Rating)</t>
+  </si>
+  <si>
+    <t>lock type (panic bar)</t>
+  </si>
+  <si>
+    <t>lock type (panic Bar)</t>
+  </si>
+  <si>
+    <t>Mustaqim Extra Large Doors</t>
+  </si>
+  <si>
+    <t>China Customised Doors</t>
+  </si>
+  <si>
+    <t>Client Doors Not Covered</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -395,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -458,16 +503,21 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -483,10 +533,6 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,7 +805,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -972,7 +1018,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
@@ -989,31 +1035,31 @@
       <c r="B1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="45" t="s">
         <v>1</v>
       </c>
       <c r="I3" s="19" t="s">
@@ -1024,13 +1070,13 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
       <c r="I4" t="s">
         <v>46</v>
       </c>
@@ -1058,68 +1104,68 @@
       <c r="B6" s="16">
         <v>3</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="I6" s="43" t="s">
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="I6" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="43"/>
-      <c r="M6" s="43"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="16">
         <v>4</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="I7" s="41" t="s">
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="I7" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
     </row>
     <row r="8" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16">
         <v>5</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="I8" s="50" t="s">
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="I8" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="J8" s="50"/>
-      <c r="K8" s="50"/>
-      <c r="L8" s="50"/>
-      <c r="M8" s="50"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
       <c r="I9" s="37"/>
       <c r="J9" s="37"/>
       <c r="K9" s="37"/>
@@ -1130,11 +1176,11 @@
       <c r="B10" s="16">
         <v>7</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
       <c r="I10" s="37"/>
       <c r="J10" s="37"/>
       <c r="K10" s="37"/>
@@ -1143,11 +1189,11 @@
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="16"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
       <c r="I11" s="37"/>
       <c r="J11" s="37"/>
       <c r="K11" s="37"/>
@@ -1158,19 +1204,19 @@
       <c r="B12" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="38" t="s">
+      <c r="E12" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="38" t="s">
+      <c r="F12" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="45" t="s">
         <v>1</v>
       </c>
       <c r="I12" s="37"/>
@@ -1183,32 +1229,32 @@
       <c r="B13" s="16">
         <v>1</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="I13" s="49" t="s">
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="I13" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="J13" s="49"/>
-      <c r="K13" s="49"/>
-      <c r="L13" s="49"/>
-      <c r="M13" s="49"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="44"/>
+      <c r="M13" s="44"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="16">
         <v>2</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
       <c r="I14" t="s">
         <v>51</v>
       </c>
@@ -1217,13 +1263,13 @@
       <c r="B15" s="16">
         <v>3</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
       <c r="I15" t="s">
         <v>52</v>
       </c>
@@ -1232,11 +1278,11 @@
       <c r="B16" s="16">
         <v>4</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
       <c r="I16" s="37" t="s">
         <v>53</v>
       </c>
@@ -1245,11 +1291,11 @@
       <c r="B17" s="16">
         <v>5</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
       <c r="I17" t="s">
         <v>54</v>
       </c>
@@ -1258,11 +1304,11 @@
       <c r="B18" s="20">
         <v>6</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
       <c r="I18" t="s">
         <v>55</v>
       </c>
@@ -1271,33 +1317,33 @@
       <c r="B19" s="16">
         <v>7</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
       <c r="I19" s="37" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="16"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
       <c r="I20" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="16"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
       <c r="I21" t="s">
         <v>58</v>
       </c>
@@ -1319,6 +1365,23 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="I13:M13"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="C10:G10"/>
@@ -1327,23 +1390,6 @@
     <mergeCell ref="I6:M6"/>
     <mergeCell ref="I7:M7"/>
     <mergeCell ref="I8:M8"/>
-    <mergeCell ref="I13:M13"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="C7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1351,6 +1397,100 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
@@ -1371,15 +1511,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="18" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="44"/>
+      <c r="B1" s="47"/>
       <c r="C1" s="25"/>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="44"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
@@ -1497,20 +1637,20 @@
       <c r="E10" s="29"/>
     </row>
     <row r="11" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="47"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="50"/>
     </row>
     <row r="12" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="47"/>
+      <c r="A12" s="51"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="50"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="28"/>

</xml_diff>